<commit_message>
add federal tax data
</commit_message>
<xml_diff>
--- a/data/Steuertarife.xlsx
+++ b/data/Steuertarife.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\PensionTools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50BDDE7-4362-4D29-853D-1B947737469D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CDD4D9-B37A-462F-B60E-E9AB641D47BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4115" yWindow="2820" windowWidth="14400" windowHeight="7380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Staatssteuer" sheetId="1" r:id="rId1"/>
+    <sheet name="Bundessteuer" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
   <si>
     <t>Jahr</t>
   </si>
@@ -371,8 +372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -725,4 +726,597 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9101B908-17CD-4F9F-B222-CF0DA0451907}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="7" max="7" width="19.58984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>2012</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>17800</v>
+      </c>
+      <c r="E2">
+        <v>25.41</v>
+      </c>
+      <c r="F2">
+        <v>0.77</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>2012</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>31700</v>
+      </c>
+      <c r="E3">
+        <v>132.53</v>
+      </c>
+      <c r="F3">
+        <v>0.88</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>41500</v>
+      </c>
+      <c r="E4">
+        <v>220.54</v>
+      </c>
+      <c r="F4">
+        <v>2.64</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>2012</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>55300</v>
+      </c>
+      <c r="E5">
+        <v>585.16999999999996</v>
+      </c>
+      <c r="F5">
+        <v>2.97</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>2012</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>72600</v>
+      </c>
+      <c r="E6">
+        <v>1101.94</v>
+      </c>
+      <c r="F6">
+        <v>5.94</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>2012</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>78200</v>
+      </c>
+      <c r="E7">
+        <v>1435.2</v>
+      </c>
+      <c r="F7">
+        <v>6.6</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A8">
+        <v>2012</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>103700</v>
+      </c>
+      <c r="E8">
+        <v>3120.4</v>
+      </c>
+      <c r="F8">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A9">
+        <v>2012</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>134700</v>
+      </c>
+      <c r="E9">
+        <v>5850.6</v>
+      </c>
+      <c r="F9">
+        <v>11</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A10">
+        <v>2012</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>176100</v>
+      </c>
+      <c r="E10">
+        <v>10406.799999999999</v>
+      </c>
+      <c r="F10">
+        <v>13.2</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A11">
+        <v>2012</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>755300</v>
+      </c>
+      <c r="E11">
+        <v>86859.5</v>
+      </c>
+      <c r="F11">
+        <v>11.5</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A12">
+        <v>2012</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>30800</v>
+      </c>
+      <c r="E12">
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A13">
+        <v>2012</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>51000</v>
+      </c>
+      <c r="E13">
+        <v>228</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A14">
+        <v>2012</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>58500</v>
+      </c>
+      <c r="E14">
+        <v>379</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A15">
+        <v>2012</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>75400</v>
+      </c>
+      <c r="E15">
+        <v>887</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A16">
+        <v>2012</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>90400</v>
+      </c>
+      <c r="E16">
+        <v>1488</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A17">
+        <v>2012</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>103500</v>
+      </c>
+      <c r="E17">
+        <v>2144</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A18">
+        <v>2012</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>114800</v>
+      </c>
+      <c r="E18">
+        <v>2823</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+      <c r="G18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A19">
+        <v>2012</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>124300</v>
+      </c>
+      <c r="E19">
+        <v>3489</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A20">
+        <v>2012</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>131800</v>
+      </c>
+      <c r="E20">
+        <v>4090</v>
+      </c>
+      <c r="F20">
+        <v>9</v>
+      </c>
+      <c r="G20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A21">
+        <v>2012</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>137400</v>
+      </c>
+      <c r="E21">
+        <v>4595</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A22">
+        <v>2012</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>141300</v>
+      </c>
+      <c r="E22">
+        <v>4986</v>
+      </c>
+      <c r="F22">
+        <v>11</v>
+      </c>
+      <c r="G22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A23">
+        <v>2012</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>143200</v>
+      </c>
+      <c r="E23">
+        <v>5196</v>
+      </c>
+      <c r="F23">
+        <v>12</v>
+      </c>
+      <c r="G23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A24">
+        <v>2012</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>145100</v>
+      </c>
+      <c r="E24">
+        <v>5425</v>
+      </c>
+      <c r="F24">
+        <v>13</v>
+      </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A25">
+        <v>2012</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>895900</v>
+      </c>
+      <c r="E25">
+        <v>103028.5</v>
+      </c>
+      <c r="F25">
+        <v>11.5</v>
+      </c>
+      <c r="G25">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add new tariff type single
</commit_message>
<xml_diff>
--- a/data/Steuertarife.xlsx
+++ b/data/Steuertarife.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\PensionTools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CDD4D9-B37A-462F-B60E-E9AB641D47BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5718EFC9-785D-4731-9E1C-D5108B04CC27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4115" yWindow="2820" windowWidth="14400" windowHeight="7380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4115" yWindow="2820" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staatssteuer" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="9">
   <si>
     <t>Jahr</t>
   </si>
@@ -370,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -425,7 +425,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>13500</v>
+        <v>6700</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -451,10 +451,10 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>19600</v>
+        <v>11400</v>
       </c>
       <c r="F3">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -477,10 +477,10 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>27300</v>
+        <v>16100</v>
       </c>
       <c r="F4">
-        <v>353</v>
+        <v>235</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -503,10 +503,10 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>36700</v>
+        <v>23700</v>
       </c>
       <c r="F5">
-        <v>729</v>
+        <v>539</v>
       </c>
       <c r="G5">
         <v>5</v>
@@ -529,10 +529,10 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>47400</v>
+        <v>33000</v>
       </c>
       <c r="F6">
-        <v>1264</v>
+        <v>1004</v>
       </c>
       <c r="G6">
         <v>6</v>
@@ -555,10 +555,10 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>61300</v>
+        <v>43700</v>
       </c>
       <c r="F7">
-        <v>2098</v>
+        <v>1646</v>
       </c>
       <c r="G7">
         <v>7</v>
@@ -581,10 +581,10 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>92100</v>
+        <v>56100</v>
       </c>
       <c r="F8">
-        <v>4254</v>
+        <v>2514</v>
       </c>
       <c r="G8">
         <v>8</v>
@@ -607,10 +607,10 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>122900</v>
+        <v>73000</v>
       </c>
       <c r="F9">
-        <v>6718</v>
+        <v>3866</v>
       </c>
       <c r="G9">
         <v>9</v>
@@ -633,10 +633,10 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>169300</v>
+        <v>105500</v>
       </c>
       <c r="F10">
-        <v>10894</v>
+        <v>6791</v>
       </c>
       <c r="G10">
         <v>10</v>
@@ -659,10 +659,10 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>224700</v>
+        <v>137700</v>
       </c>
       <c r="F11">
-        <v>16434</v>
+        <v>10011</v>
       </c>
       <c r="G11">
         <v>11</v>
@@ -685,10 +685,10 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>284800</v>
+        <v>188700</v>
       </c>
       <c r="F12">
-        <v>23045</v>
+        <v>15621</v>
       </c>
       <c r="G12">
         <v>12</v>
@@ -711,15 +711,327 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>354100</v>
+        <v>254900</v>
       </c>
       <c r="F13">
-        <v>31361</v>
+        <v>23565</v>
       </c>
       <c r="G13">
         <v>13</v>
       </c>
       <c r="H13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A14">
+        <v>2018</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>13500</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A15">
+        <v>2018</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>19600</v>
+      </c>
+      <c r="F15">
+        <v>122</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A16">
+        <v>2018</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>27300</v>
+      </c>
+      <c r="F16">
+        <v>353</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A17">
+        <v>2018</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>36700</v>
+      </c>
+      <c r="F17">
+        <v>729</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A18">
+        <v>2018</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>47400</v>
+      </c>
+      <c r="F18">
+        <v>1264</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A19">
+        <v>2018</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>61300</v>
+      </c>
+      <c r="F19">
+        <v>2098</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A20">
+        <v>2018</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>92100</v>
+      </c>
+      <c r="F20">
+        <v>4254</v>
+      </c>
+      <c r="G20">
+        <v>8</v>
+      </c>
+      <c r="H20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A21">
+        <v>2018</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>122900</v>
+      </c>
+      <c r="F21">
+        <v>6718</v>
+      </c>
+      <c r="G21">
+        <v>9</v>
+      </c>
+      <c r="H21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A22">
+        <v>2018</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>169300</v>
+      </c>
+      <c r="F22">
+        <v>10894</v>
+      </c>
+      <c r="G22">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A23">
+        <v>2018</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>224700</v>
+      </c>
+      <c r="F23">
+        <v>16434</v>
+      </c>
+      <c r="G23">
+        <v>11</v>
+      </c>
+      <c r="H23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A24">
+        <v>2018</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>284800</v>
+      </c>
+      <c r="F24">
+        <v>23045</v>
+      </c>
+      <c r="G24">
+        <v>12</v>
+      </c>
+      <c r="H24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A25">
+        <v>2018</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>354100</v>
+      </c>
+      <c r="F25">
+        <v>31361</v>
+      </c>
+      <c r="G25">
+        <v>13</v>
+      </c>
+      <c r="H25">
         <v>100</v>
       </c>
     </row>
@@ -732,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9101B908-17CD-4F9F-B222-CF0DA0451907}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>

</xml_diff>

<commit_message>
add wealth tax tariff
</commit_message>
<xml_diff>
--- a/data/Steuertarife.xlsx
+++ b/data/Steuertarife.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\PensionTools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5718EFC9-785D-4731-9E1C-D5108B04CC27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3CC5C1-600C-49FB-AAF0-5A8B762D7B7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4115" yWindow="2820" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="9">
   <si>
     <t>Jahr</t>
   </si>
@@ -370,19 +370,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="3" max="3" width="15.2265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.2265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.453125" customWidth="1"/>
+    <col min="4" max="4" width="4.6328125" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" customWidth="1"/>
     <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.58984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" customWidth="1"/>
+    <col min="8" max="8" width="13.40625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.75">
@@ -1033,6 +1034,318 @@
       </c>
       <c r="H25">
         <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A26">
+        <v>2018</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>77000</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0.5</v>
+      </c>
+      <c r="H26">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A27">
+        <v>2018</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>308000</v>
+      </c>
+      <c r="F27">
+        <v>115.5</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A28">
+        <v>2018</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>694000</v>
+      </c>
+      <c r="F28">
+        <v>501.5</v>
+      </c>
+      <c r="G28">
+        <v>1.5</v>
+      </c>
+      <c r="H28">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A29">
+        <v>2018</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1310000</v>
+      </c>
+      <c r="F29">
+        <v>1425.5</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A30">
+        <v>2018</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>2235000</v>
+      </c>
+      <c r="F30">
+        <v>3275.5</v>
+      </c>
+      <c r="G30">
+        <v>2.5</v>
+      </c>
+      <c r="H30">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A31">
+        <v>2018</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>3158000</v>
+      </c>
+      <c r="F31">
+        <v>5583</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A32">
+        <v>2018</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>154000</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0.5</v>
+      </c>
+      <c r="H32">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A33">
+        <v>2018</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>385000</v>
+      </c>
+      <c r="F33">
+        <v>115.5</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A34">
+        <v>2018</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>770000</v>
+      </c>
+      <c r="F34">
+        <v>500.5</v>
+      </c>
+      <c r="G34">
+        <v>1.5</v>
+      </c>
+      <c r="H34">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A35">
+        <v>2018</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>1386000</v>
+      </c>
+      <c r="F35">
+        <v>1424.5</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A36">
+        <v>2018</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>2311000</v>
+      </c>
+      <c r="F36">
+        <v>3274.5</v>
+      </c>
+      <c r="G36">
+        <v>2.5</v>
+      </c>
+      <c r="H36">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A37">
+        <v>2018</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>3235000</v>
+      </c>
+      <c r="F37">
+        <v>5584.5</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calculate federal tax unit test successfully
</commit_message>
<xml_diff>
--- a/data/Steuertarife.xlsx
+++ b/data/Steuertarife.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\PensionTools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC4EC5B-D0E8-4E34-A7AF-582296FCE22D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E059036-45C9-4962-A4D2-A858B2D2F5F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="9">
   <si>
     <t>Jahr</t>
   </si>
@@ -1355,41 +1355,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9101B908-17CD-4F9F-B222-CF0DA0451907}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:A49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="7" max="7" width="19.58984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.58984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>2012</v>
       </c>
@@ -1397,22 +1394,19 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>17800</v>
       </c>
       <c r="D2">
-        <v>17800</v>
+        <v>25.41</v>
       </c>
       <c r="E2">
-        <v>25.41</v>
+        <v>0.77</v>
       </c>
       <c r="F2">
-        <v>0.77</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>2012</v>
       </c>
@@ -1420,22 +1414,19 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>31700</v>
       </c>
       <c r="D3">
-        <v>31700</v>
+        <v>132.53</v>
       </c>
       <c r="E3">
-        <v>132.53</v>
+        <v>0.88</v>
       </c>
       <c r="F3">
-        <v>0.88</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -1443,22 +1434,19 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>41500</v>
       </c>
       <c r="D4">
-        <v>41500</v>
+        <v>220.54</v>
       </c>
       <c r="E4">
-        <v>220.54</v>
+        <v>2.64</v>
       </c>
       <c r="F4">
-        <v>2.64</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>2012</v>
       </c>
@@ -1466,22 +1454,19 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>55300</v>
       </c>
       <c r="D5">
-        <v>55300</v>
+        <v>585.16999999999996</v>
       </c>
       <c r="E5">
-        <v>585.16999999999996</v>
+        <v>2.97</v>
       </c>
       <c r="F5">
-        <v>2.97</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>2012</v>
       </c>
@@ -1489,22 +1474,19 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>72600</v>
       </c>
       <c r="D6">
-        <v>72600</v>
+        <v>1101.94</v>
       </c>
       <c r="E6">
-        <v>1101.94</v>
+        <v>5.94</v>
       </c>
       <c r="F6">
-        <v>5.94</v>
-      </c>
-      <c r="G6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>2012</v>
       </c>
@@ -1512,22 +1494,19 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>78200</v>
       </c>
       <c r="D7">
-        <v>78200</v>
+        <v>1435.2</v>
       </c>
       <c r="E7">
-        <v>1435.2</v>
+        <v>6.6</v>
       </c>
       <c r="F7">
-        <v>6.6</v>
-      </c>
-      <c r="G7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>2012</v>
       </c>
@@ -1535,22 +1514,19 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>103700</v>
       </c>
       <c r="D8">
-        <v>103700</v>
+        <v>3120.4</v>
       </c>
       <c r="E8">
-        <v>3120.4</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F8">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="G8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>2012</v>
       </c>
@@ -1558,22 +1534,19 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>134700</v>
       </c>
       <c r="D9">
-        <v>134700</v>
+        <v>5850.6</v>
       </c>
       <c r="E9">
-        <v>5850.6</v>
+        <v>11</v>
       </c>
       <c r="F9">
-        <v>11</v>
-      </c>
-      <c r="G9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>2012</v>
       </c>
@@ -1581,22 +1554,19 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>176100</v>
       </c>
       <c r="D10">
-        <v>176100</v>
+        <v>10406.799999999999</v>
       </c>
       <c r="E10">
-        <v>10406.799999999999</v>
+        <v>13.2</v>
       </c>
       <c r="F10">
-        <v>13.2</v>
-      </c>
-      <c r="G10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>2012</v>
       </c>
@@ -1604,892 +1574,775 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>755300</v>
       </c>
       <c r="D11">
-        <v>755300</v>
+        <v>86859.5</v>
       </c>
       <c r="E11">
-        <v>86859.5</v>
+        <v>11.5</v>
       </c>
       <c r="F11">
-        <v>11.5</v>
-      </c>
-      <c r="G11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>2012</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>30800</v>
       </c>
       <c r="D12">
-        <v>30800</v>
+        <v>25</v>
       </c>
       <c r="E12">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>2012</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>51000</v>
       </c>
       <c r="D13">
-        <v>51000</v>
+        <v>228</v>
       </c>
       <c r="E13">
-        <v>228</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="G13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>2012</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>58500</v>
       </c>
       <c r="D14">
-        <v>58500</v>
+        <v>379</v>
       </c>
       <c r="E14">
-        <v>379</v>
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A15">
         <v>2012</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>75400</v>
       </c>
       <c r="D15">
-        <v>75400</v>
+        <v>887</v>
       </c>
       <c r="E15">
-        <v>887</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>4</v>
-      </c>
-      <c r="G15">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A16">
         <v>2012</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>90400</v>
       </c>
       <c r="D16">
-        <v>90400</v>
+        <v>1488</v>
       </c>
       <c r="E16">
-        <v>1488</v>
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>5</v>
-      </c>
-      <c r="G16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A17">
         <v>2012</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>103500</v>
       </c>
       <c r="D17">
-        <v>103500</v>
+        <v>2144</v>
       </c>
       <c r="E17">
-        <v>2144</v>
+        <v>6</v>
       </c>
       <c r="F17">
-        <v>6</v>
-      </c>
-      <c r="G17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A18">
         <v>2012</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>114800</v>
       </c>
       <c r="D18">
-        <v>114800</v>
+        <v>2823</v>
       </c>
       <c r="E18">
-        <v>2823</v>
+        <v>7</v>
       </c>
       <c r="F18">
-        <v>7</v>
-      </c>
-      <c r="G18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A19">
         <v>2012</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>124300</v>
       </c>
       <c r="D19">
-        <v>124300</v>
+        <v>3489</v>
       </c>
       <c r="E19">
-        <v>3489</v>
+        <v>8</v>
       </c>
       <c r="F19">
-        <v>8</v>
-      </c>
-      <c r="G19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A20">
         <v>2012</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>131800</v>
       </c>
       <c r="D20">
-        <v>131800</v>
+        <v>4090</v>
       </c>
       <c r="E20">
-        <v>4090</v>
+        <v>9</v>
       </c>
       <c r="F20">
-        <v>9</v>
-      </c>
-      <c r="G20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A21">
         <v>2012</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>137400</v>
       </c>
       <c r="D21">
-        <v>137400</v>
+        <v>4595</v>
       </c>
       <c r="E21">
-        <v>4595</v>
+        <v>10</v>
       </c>
       <c r="F21">
-        <v>10</v>
-      </c>
-      <c r="G21">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A22">
         <v>2012</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>141300</v>
       </c>
       <c r="D22">
-        <v>141300</v>
+        <v>4986</v>
       </c>
       <c r="E22">
-        <v>4986</v>
+        <v>11</v>
       </c>
       <c r="F22">
-        <v>11</v>
-      </c>
-      <c r="G22">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A23">
         <v>2012</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>143200</v>
       </c>
       <c r="D23">
-        <v>143200</v>
+        <v>5196</v>
       </c>
       <c r="E23">
-        <v>5196</v>
+        <v>12</v>
       </c>
       <c r="F23">
-        <v>12</v>
-      </c>
-      <c r="G23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A24">
         <v>2012</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>145100</v>
       </c>
       <c r="D24">
-        <v>145100</v>
+        <v>5425</v>
       </c>
       <c r="E24">
-        <v>5425</v>
+        <v>13</v>
       </c>
       <c r="F24">
-        <v>13</v>
-      </c>
-      <c r="G24">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A25">
         <v>2012</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>895900</v>
       </c>
       <c r="D25">
+        <v>103028.5</v>
+      </c>
+      <c r="E25">
+        <v>11.5</v>
+      </c>
+      <c r="F25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A26">
+        <v>2018</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>17800</v>
+      </c>
+      <c r="D26">
+        <v>25.41</v>
+      </c>
+      <c r="E26">
+        <v>0.77</v>
+      </c>
+      <c r="F26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A27">
+        <v>2018</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>31700</v>
+      </c>
+      <c r="D27">
+        <v>132.53</v>
+      </c>
+      <c r="E27">
+        <v>0.88</v>
+      </c>
+      <c r="F27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A28">
+        <v>2018</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>41500</v>
+      </c>
+      <c r="D28">
+        <v>220.54</v>
+      </c>
+      <c r="E28">
+        <v>2.64</v>
+      </c>
+      <c r="F28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A29">
+        <v>2018</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>55300</v>
+      </c>
+      <c r="D29">
+        <v>585.16999999999996</v>
+      </c>
+      <c r="E29">
+        <v>2.97</v>
+      </c>
+      <c r="F29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A30">
+        <v>2018</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>72600</v>
+      </c>
+      <c r="D30">
+        <v>1101.94</v>
+      </c>
+      <c r="E30">
+        <v>5.94</v>
+      </c>
+      <c r="F30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A31">
+        <v>2018</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>78200</v>
+      </c>
+      <c r="D31">
+        <v>1435.2</v>
+      </c>
+      <c r="E31">
+        <v>6.6</v>
+      </c>
+      <c r="F31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A32">
+        <v>2018</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>103700</v>
+      </c>
+      <c r="D32">
+        <v>3120.4</v>
+      </c>
+      <c r="E32">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A33">
+        <v>2018</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>134700</v>
+      </c>
+      <c r="D33">
+        <v>5850.6</v>
+      </c>
+      <c r="E33">
+        <v>11</v>
+      </c>
+      <c r="F33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A34">
+        <v>2018</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>176100</v>
+      </c>
+      <c r="D34">
+        <v>10406.799999999999</v>
+      </c>
+      <c r="E34">
+        <v>13.2</v>
+      </c>
+      <c r="F34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A35">
+        <v>2018</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>755300</v>
+      </c>
+      <c r="D35">
+        <v>86859.5</v>
+      </c>
+      <c r="E35">
+        <v>11.5</v>
+      </c>
+      <c r="F35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A36">
+        <v>2018</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>30800</v>
+      </c>
+      <c r="D36">
+        <v>25</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A37">
+        <v>2018</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>51000</v>
+      </c>
+      <c r="D37">
+        <v>228</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A38">
+        <v>2018</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>58500</v>
+      </c>
+      <c r="D38">
+        <v>379</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A39">
+        <v>2018</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>75400</v>
+      </c>
+      <c r="D39">
+        <v>887</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A40">
+        <v>2018</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>90400</v>
+      </c>
+      <c r="D40">
+        <v>1488</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A41">
+        <v>2018</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>103500</v>
+      </c>
+      <c r="D41">
+        <v>2144</v>
+      </c>
+      <c r="E41">
+        <v>6</v>
+      </c>
+      <c r="F41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A42">
+        <v>2018</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>114800</v>
+      </c>
+      <c r="D42">
+        <v>2823</v>
+      </c>
+      <c r="E42">
+        <v>7</v>
+      </c>
+      <c r="F42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A43">
+        <v>2018</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>124300</v>
+      </c>
+      <c r="D43">
+        <v>3489</v>
+      </c>
+      <c r="E43">
+        <v>8</v>
+      </c>
+      <c r="F43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A44">
+        <v>2018</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>131800</v>
+      </c>
+      <c r="D44">
+        <v>4090</v>
+      </c>
+      <c r="E44">
+        <v>9</v>
+      </c>
+      <c r="F44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A45">
+        <v>2018</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>137400</v>
+      </c>
+      <c r="D45">
+        <v>4595</v>
+      </c>
+      <c r="E45">
+        <v>10</v>
+      </c>
+      <c r="F45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A46">
+        <v>2018</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>141300</v>
+      </c>
+      <c r="D46">
+        <v>4986</v>
+      </c>
+      <c r="E46">
+        <v>11</v>
+      </c>
+      <c r="F46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A47">
+        <v>2018</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>143200</v>
+      </c>
+      <c r="D47">
+        <v>5196</v>
+      </c>
+      <c r="E47">
+        <v>12</v>
+      </c>
+      <c r="F47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A48">
+        <v>2018</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>145100</v>
+      </c>
+      <c r="D48">
+        <v>5425</v>
+      </c>
+      <c r="E48">
+        <v>13</v>
+      </c>
+      <c r="F48">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A49">
+        <v>2018</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
         <v>895900</v>
       </c>
-      <c r="E25">
+      <c r="D49">
         <v>103028.5</v>
       </c>
-      <c r="F25">
+      <c r="E49">
         <v>11.5</v>
       </c>
-      <c r="G25">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A26">
-        <v>2018</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>17800</v>
-      </c>
-      <c r="E26">
-        <v>25.41</v>
-      </c>
-      <c r="F26">
-        <v>0.77</v>
-      </c>
-      <c r="G26">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A27">
-        <v>2018</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>31700</v>
-      </c>
-      <c r="E27">
-        <v>132.53</v>
-      </c>
-      <c r="F27">
-        <v>0.88</v>
-      </c>
-      <c r="G27">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A28">
-        <v>2018</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28">
-        <v>41500</v>
-      </c>
-      <c r="E28">
-        <v>220.54</v>
-      </c>
-      <c r="F28">
-        <v>2.64</v>
-      </c>
-      <c r="G28">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A29">
-        <v>2018</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>55300</v>
-      </c>
-      <c r="E29">
-        <v>585.16999999999996</v>
-      </c>
-      <c r="F29">
-        <v>2.97</v>
-      </c>
-      <c r="G29">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A30">
-        <v>2018</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <v>72600</v>
-      </c>
-      <c r="E30">
-        <v>1101.94</v>
-      </c>
-      <c r="F30">
-        <v>5.94</v>
-      </c>
-      <c r="G30">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A31">
-        <v>2018</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>78200</v>
-      </c>
-      <c r="E31">
-        <v>1435.2</v>
-      </c>
-      <c r="F31">
-        <v>6.6</v>
-      </c>
-      <c r="G31">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A32">
-        <v>2018</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>103700</v>
-      </c>
-      <c r="E32">
-        <v>3120.4</v>
-      </c>
-      <c r="F32">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="G32">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A33">
-        <v>2018</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>134700</v>
-      </c>
-      <c r="E33">
-        <v>5850.6</v>
-      </c>
-      <c r="F33">
-        <v>11</v>
-      </c>
-      <c r="G33">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A34">
-        <v>2018</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>176100</v>
-      </c>
-      <c r="E34">
-        <v>10406.799999999999</v>
-      </c>
-      <c r="F34">
-        <v>13.2</v>
-      </c>
-      <c r="G34">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A35">
-        <v>2018</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>755300</v>
-      </c>
-      <c r="E35">
-        <v>86859.5</v>
-      </c>
-      <c r="F35">
-        <v>11.5</v>
-      </c>
-      <c r="G35">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A36">
-        <v>2018</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36">
-        <v>30800</v>
-      </c>
-      <c r="E36">
-        <v>25</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A37">
-        <v>2018</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37">
-        <v>51000</v>
-      </c>
-      <c r="E37">
-        <v>228</v>
-      </c>
-      <c r="F37">
-        <v>2</v>
-      </c>
-      <c r="G37">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A38">
-        <v>2018</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38">
-        <v>58500</v>
-      </c>
-      <c r="E38">
-        <v>379</v>
-      </c>
-      <c r="F38">
-        <v>3</v>
-      </c>
-      <c r="G38">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A39">
-        <v>2018</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-      <c r="D39">
-        <v>75400</v>
-      </c>
-      <c r="E39">
-        <v>887</v>
-      </c>
-      <c r="F39">
-        <v>4</v>
-      </c>
-      <c r="G39">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A40">
-        <v>2018</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40">
-        <v>90400</v>
-      </c>
-      <c r="E40">
-        <v>1488</v>
-      </c>
-      <c r="F40">
-        <v>5</v>
-      </c>
-      <c r="G40">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A41">
-        <v>2018</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
-      <c r="D41">
-        <v>103500</v>
-      </c>
-      <c r="E41">
-        <v>2144</v>
-      </c>
-      <c r="F41">
-        <v>6</v>
-      </c>
-      <c r="G41">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A42">
-        <v>2018</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42">
-        <v>114800</v>
-      </c>
-      <c r="E42">
-        <v>2823</v>
-      </c>
-      <c r="F42">
-        <v>7</v>
-      </c>
-      <c r="G42">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A43">
-        <v>2018</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43">
-        <v>124300</v>
-      </c>
-      <c r="E43">
-        <v>3489</v>
-      </c>
-      <c r="F43">
-        <v>8</v>
-      </c>
-      <c r="G43">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A44">
-        <v>2018</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-      <c r="D44">
-        <v>131800</v>
-      </c>
-      <c r="E44">
-        <v>4090</v>
-      </c>
-      <c r="F44">
-        <v>9</v>
-      </c>
-      <c r="G44">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A45">
-        <v>2018</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45">
-        <v>137400</v>
-      </c>
-      <c r="E45">
-        <v>4595</v>
-      </c>
-      <c r="F45">
-        <v>10</v>
-      </c>
-      <c r="G45">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A46">
-        <v>2018</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46">
-        <v>141300</v>
-      </c>
-      <c r="E46">
-        <v>4986</v>
-      </c>
-      <c r="F46">
-        <v>11</v>
-      </c>
-      <c r="G46">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A47">
-        <v>2018</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <v>2</v>
-      </c>
-      <c r="D47">
-        <v>143200</v>
-      </c>
-      <c r="E47">
-        <v>5196</v>
-      </c>
-      <c r="F47">
-        <v>12</v>
-      </c>
-      <c r="G47">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A48">
-        <v>2018</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48">
-        <v>145100</v>
-      </c>
-      <c r="E48">
-        <v>5425</v>
-      </c>
-      <c r="F48">
-        <v>13</v>
-      </c>
-      <c r="G48">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A49">
-        <v>2018</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-      <c r="D49">
-        <v>895900</v>
-      </c>
-      <c r="E49">
-        <v>103028.5</v>
-      </c>
       <c r="F49">
-        <v>11.5</v>
-      </c>
-      <c r="G49">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new 2019 data for Zürich
</commit_message>
<xml_diff>
--- a/data/Steuertarife.xlsx
+++ b/data/Steuertarife.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\PensionTools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E059036-45C9-4962-A4D2-A858B2D2F5F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E93A721-2073-4645-B495-DFE32F8083B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="9">
   <si>
     <t>Jahr</t>
   </si>
@@ -370,16 +370,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="3" max="3" width="5.453125" customWidth="1"/>
-    <col min="4" max="4" width="4.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.81640625" customWidth="1"/>
     <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5" customWidth="1"/>
@@ -1348,6 +1348,942 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A38">
+        <v>2019</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>6700</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A39">
+        <v>2019</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>11400</v>
+      </c>
+      <c r="F39">
+        <v>94</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A40">
+        <v>2019</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>16100</v>
+      </c>
+      <c r="F40">
+        <v>235</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A41">
+        <v>2019</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>23700</v>
+      </c>
+      <c r="F41">
+        <v>539</v>
+      </c>
+      <c r="G41">
+        <v>5</v>
+      </c>
+      <c r="H41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A42">
+        <v>2019</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>33000</v>
+      </c>
+      <c r="F42">
+        <v>1004</v>
+      </c>
+      <c r="G42">
+        <v>6</v>
+      </c>
+      <c r="H42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A43">
+        <v>2019</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>43700</v>
+      </c>
+      <c r="F43">
+        <v>1646</v>
+      </c>
+      <c r="G43">
+        <v>7</v>
+      </c>
+      <c r="H43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A44">
+        <v>2019</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>56100</v>
+      </c>
+      <c r="F44">
+        <v>2514</v>
+      </c>
+      <c r="G44">
+        <v>8</v>
+      </c>
+      <c r="H44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A45">
+        <v>2019</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>73000</v>
+      </c>
+      <c r="F45">
+        <v>3866</v>
+      </c>
+      <c r="G45">
+        <v>9</v>
+      </c>
+      <c r="H45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A46">
+        <v>2019</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>105500</v>
+      </c>
+      <c r="F46">
+        <v>6791</v>
+      </c>
+      <c r="G46">
+        <v>10</v>
+      </c>
+      <c r="H46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A47">
+        <v>2019</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>137700</v>
+      </c>
+      <c r="F47">
+        <v>10011</v>
+      </c>
+      <c r="G47">
+        <v>11</v>
+      </c>
+      <c r="H47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A48">
+        <v>2019</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>188700</v>
+      </c>
+      <c r="F48">
+        <v>15621</v>
+      </c>
+      <c r="G48">
+        <v>12</v>
+      </c>
+      <c r="H48">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A49">
+        <v>2019</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>254900</v>
+      </c>
+      <c r="F49">
+        <v>23565</v>
+      </c>
+      <c r="G49">
+        <v>13</v>
+      </c>
+      <c r="H49">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A50">
+        <v>2019</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>13500</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
+      <c r="H50">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A51">
+        <v>2019</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51">
+        <v>19600</v>
+      </c>
+      <c r="F51">
+        <v>122</v>
+      </c>
+      <c r="G51">
+        <v>3</v>
+      </c>
+      <c r="H51">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A52">
+        <v>2019</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>27300</v>
+      </c>
+      <c r="F52">
+        <v>353</v>
+      </c>
+      <c r="G52">
+        <v>4</v>
+      </c>
+      <c r="H52">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A53">
+        <v>2019</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>36700</v>
+      </c>
+      <c r="F53">
+        <v>729</v>
+      </c>
+      <c r="G53">
+        <v>5</v>
+      </c>
+      <c r="H53">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A54">
+        <v>2019</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>47400</v>
+      </c>
+      <c r="F54">
+        <v>1264</v>
+      </c>
+      <c r="G54">
+        <v>6</v>
+      </c>
+      <c r="H54">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A55">
+        <v>2019</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>61300</v>
+      </c>
+      <c r="F55">
+        <v>2098</v>
+      </c>
+      <c r="G55">
+        <v>7</v>
+      </c>
+      <c r="H55">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A56">
+        <v>2019</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>92100</v>
+      </c>
+      <c r="F56">
+        <v>4254</v>
+      </c>
+      <c r="G56">
+        <v>8</v>
+      </c>
+      <c r="H56">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A57">
+        <v>2019</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>122900</v>
+      </c>
+      <c r="F57">
+        <v>6718</v>
+      </c>
+      <c r="G57">
+        <v>9</v>
+      </c>
+      <c r="H57">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A58">
+        <v>2019</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>169300</v>
+      </c>
+      <c r="F58">
+        <v>10894</v>
+      </c>
+      <c r="G58">
+        <v>10</v>
+      </c>
+      <c r="H58">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A59">
+        <v>2019</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>224700</v>
+      </c>
+      <c r="F59">
+        <v>16434</v>
+      </c>
+      <c r="G59">
+        <v>11</v>
+      </c>
+      <c r="H59">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A60">
+        <v>2019</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>284800</v>
+      </c>
+      <c r="F60">
+        <v>23045</v>
+      </c>
+      <c r="G60">
+        <v>12</v>
+      </c>
+      <c r="H60">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A61">
+        <v>2019</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>354100</v>
+      </c>
+      <c r="F61">
+        <v>31361</v>
+      </c>
+      <c r="G61">
+        <v>13</v>
+      </c>
+      <c r="H61">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A62">
+        <v>2019</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>77000</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0.5</v>
+      </c>
+      <c r="H62">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A63">
+        <v>2019</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>308000</v>
+      </c>
+      <c r="F63">
+        <v>115.5</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A64">
+        <v>2019</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>694000</v>
+      </c>
+      <c r="F64">
+        <v>501.5</v>
+      </c>
+      <c r="G64">
+        <v>1.5</v>
+      </c>
+      <c r="H64">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A65">
+        <v>2019</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1310000</v>
+      </c>
+      <c r="F65">
+        <v>1425.5</v>
+      </c>
+      <c r="G65">
+        <v>2</v>
+      </c>
+      <c r="H65">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A66">
+        <v>2019</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>2235000</v>
+      </c>
+      <c r="F66">
+        <v>3275.5</v>
+      </c>
+      <c r="G66">
+        <v>2.5</v>
+      </c>
+      <c r="H66">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A67">
+        <v>2019</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>3158000</v>
+      </c>
+      <c r="F67">
+        <v>5583</v>
+      </c>
+      <c r="G67">
+        <v>3</v>
+      </c>
+      <c r="H67">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A68">
+        <v>2019</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>154000</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0.5</v>
+      </c>
+      <c r="H68">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A69">
+        <v>2019</v>
+      </c>
+      <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <v>385000</v>
+      </c>
+      <c r="F69">
+        <v>115.5</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A70">
+        <v>2019</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70">
+        <v>4</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <v>770000</v>
+      </c>
+      <c r="F70">
+        <v>500.5</v>
+      </c>
+      <c r="G70">
+        <v>1.5</v>
+      </c>
+      <c r="H70">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A71">
+        <v>2019</v>
+      </c>
+      <c r="B71" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <v>1386000</v>
+      </c>
+      <c r="F71">
+        <v>1424.5</v>
+      </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
+      <c r="H71">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A72">
+        <v>2019</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <v>2311000</v>
+      </c>
+      <c r="F72">
+        <v>3274.5</v>
+      </c>
+      <c r="G72">
+        <v>2.5</v>
+      </c>
+      <c r="H72">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A73">
+        <v>2019</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73">
+        <v>4</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73">
+        <v>3235000</v>
+      </c>
+      <c r="F73">
+        <v>5584.5</v>
+      </c>
+      <c r="G73">
+        <v>3</v>
+      </c>
+      <c r="H73">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1355,10 +2291,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9101B908-17CD-4F9F-B222-CF0DA0451907}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2346,6 +3282,486 @@
         <v>100</v>
       </c>
     </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A50">
+        <v>2019</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>17800</v>
+      </c>
+      <c r="D50">
+        <v>25.41</v>
+      </c>
+      <c r="E50">
+        <v>0.77</v>
+      </c>
+      <c r="F50">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A51">
+        <v>2019</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>31700</v>
+      </c>
+      <c r="D51">
+        <v>132.53</v>
+      </c>
+      <c r="E51">
+        <v>0.88</v>
+      </c>
+      <c r="F51">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A52">
+        <v>2019</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>41500</v>
+      </c>
+      <c r="D52">
+        <v>220.54</v>
+      </c>
+      <c r="E52">
+        <v>2.64</v>
+      </c>
+      <c r="F52">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A53">
+        <v>2019</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>55300</v>
+      </c>
+      <c r="D53">
+        <v>585.16999999999996</v>
+      </c>
+      <c r="E53">
+        <v>2.97</v>
+      </c>
+      <c r="F53">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A54">
+        <v>2019</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>72600</v>
+      </c>
+      <c r="D54">
+        <v>1101.94</v>
+      </c>
+      <c r="E54">
+        <v>5.94</v>
+      </c>
+      <c r="F54">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A55">
+        <v>2019</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>78200</v>
+      </c>
+      <c r="D55">
+        <v>1435.2</v>
+      </c>
+      <c r="E55">
+        <v>6.6</v>
+      </c>
+      <c r="F55">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A56">
+        <v>2019</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>103700</v>
+      </c>
+      <c r="D56">
+        <v>3120.4</v>
+      </c>
+      <c r="E56">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F56">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A57">
+        <v>2019</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>134700</v>
+      </c>
+      <c r="D57">
+        <v>5850.6</v>
+      </c>
+      <c r="E57">
+        <v>11</v>
+      </c>
+      <c r="F57">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A58">
+        <v>2019</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>176100</v>
+      </c>
+      <c r="D58">
+        <v>10406.799999999999</v>
+      </c>
+      <c r="E58">
+        <v>13.2</v>
+      </c>
+      <c r="F58">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A59">
+        <v>2019</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>755300</v>
+      </c>
+      <c r="D59">
+        <v>86859.5</v>
+      </c>
+      <c r="E59">
+        <v>11.5</v>
+      </c>
+      <c r="F59">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A60">
+        <v>2019</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <v>30800</v>
+      </c>
+      <c r="D60">
+        <v>25</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A61">
+        <v>2019</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>51000</v>
+      </c>
+      <c r="D61">
+        <v>228</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A62">
+        <v>2019</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>58500</v>
+      </c>
+      <c r="D62">
+        <v>379</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="F62">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A63">
+        <v>2019</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>75400</v>
+      </c>
+      <c r="D63">
+        <v>887</v>
+      </c>
+      <c r="E63">
+        <v>4</v>
+      </c>
+      <c r="F63">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A64">
+        <v>2019</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>90400</v>
+      </c>
+      <c r="D64">
+        <v>1488</v>
+      </c>
+      <c r="E64">
+        <v>5</v>
+      </c>
+      <c r="F64">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A65">
+        <v>2019</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65">
+        <v>103500</v>
+      </c>
+      <c r="D65">
+        <v>2144</v>
+      </c>
+      <c r="E65">
+        <v>6</v>
+      </c>
+      <c r="F65">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A66">
+        <v>2019</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66">
+        <v>114800</v>
+      </c>
+      <c r="D66">
+        <v>2823</v>
+      </c>
+      <c r="E66">
+        <v>7</v>
+      </c>
+      <c r="F66">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A67">
+        <v>2019</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67">
+        <v>124300</v>
+      </c>
+      <c r="D67">
+        <v>3489</v>
+      </c>
+      <c r="E67">
+        <v>8</v>
+      </c>
+      <c r="F67">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A68">
+        <v>2019</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <v>131800</v>
+      </c>
+      <c r="D68">
+        <v>4090</v>
+      </c>
+      <c r="E68">
+        <v>9</v>
+      </c>
+      <c r="F68">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A69">
+        <v>2019</v>
+      </c>
+      <c r="B69">
+        <v>2</v>
+      </c>
+      <c r="C69">
+        <v>137400</v>
+      </c>
+      <c r="D69">
+        <v>4595</v>
+      </c>
+      <c r="E69">
+        <v>10</v>
+      </c>
+      <c r="F69">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A70">
+        <v>2019</v>
+      </c>
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70">
+        <v>141300</v>
+      </c>
+      <c r="D70">
+        <v>4986</v>
+      </c>
+      <c r="E70">
+        <v>11</v>
+      </c>
+      <c r="F70">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A71">
+        <v>2019</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71">
+        <v>143200</v>
+      </c>
+      <c r="D71">
+        <v>5196</v>
+      </c>
+      <c r="E71">
+        <v>12</v>
+      </c>
+      <c r="F71">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A72">
+        <v>2019</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72">
+        <v>145100</v>
+      </c>
+      <c r="D72">
+        <v>5425</v>
+      </c>
+      <c r="E72">
+        <v>13</v>
+      </c>
+      <c r="F72">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A73">
+        <v>2019</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73">
+        <v>895900</v>
+      </c>
+      <c r="D73">
+        <v>103028.5</v>
+      </c>
+      <c r="E73">
+        <v>11.5</v>
+      </c>
+      <c r="F73">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add tax tariff data for canton SO
</commit_message>
<xml_diff>
--- a/data/Steuertarife.xlsx
+++ b/data/Steuertarife.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\PensionTools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182308C7-562D-4218-8893-2EA0F0600A83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC7CDEA-ED05-409F-A561-016A74DC58D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="12">
   <si>
     <t>Jahr</t>
   </si>
@@ -66,15 +68,24 @@
   <si>
     <t>SteuerfussKanton</t>
   </si>
+  <si>
+    <t>SO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -382,15 +393,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="L78" sqref="L78"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="K106" sqref="K106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="3" max="3" width="5.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.31640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
@@ -474,7 +485,7 @@
         <v>11400</v>
       </c>
       <c r="F3">
-        <f>F2+(E3-E2)*(G2/100)</f>
+        <f t="shared" ref="F3:F13" si="0">F2+(E3-E2)*(G2/100)</f>
         <v>94</v>
       </c>
       <c r="G3">
@@ -504,7 +515,7 @@
         <v>16100</v>
       </c>
       <c r="F4">
-        <f>F3+(E4-E3)*(G3/100)</f>
+        <f t="shared" si="0"/>
         <v>235</v>
       </c>
       <c r="G4">
@@ -534,7 +545,7 @@
         <v>23700</v>
       </c>
       <c r="F5">
-        <f>F4+(E5-E4)*(G4/100)</f>
+        <f t="shared" si="0"/>
         <v>539</v>
       </c>
       <c r="G5">
@@ -564,7 +575,7 @@
         <v>33000</v>
       </c>
       <c r="F6">
-        <f>F5+(E6-E5)*(G5/100)</f>
+        <f t="shared" si="0"/>
         <v>1004</v>
       </c>
       <c r="G6">
@@ -594,7 +605,7 @@
         <v>43700</v>
       </c>
       <c r="F7">
-        <f>F6+(E7-E6)*(G6/100)</f>
+        <f t="shared" si="0"/>
         <v>1646</v>
       </c>
       <c r="G7">
@@ -624,7 +635,7 @@
         <v>56100</v>
       </c>
       <c r="F8">
-        <f>F7+(E8-E7)*(G7/100)</f>
+        <f t="shared" si="0"/>
         <v>2514</v>
       </c>
       <c r="G8">
@@ -654,7 +665,7 @@
         <v>73000</v>
       </c>
       <c r="F9">
-        <f>F8+(E9-E8)*(G8/100)</f>
+        <f t="shared" si="0"/>
         <v>3866</v>
       </c>
       <c r="G9">
@@ -684,7 +695,7 @@
         <v>105500</v>
       </c>
       <c r="F10">
-        <f>F9+(E10-E9)*(G9/100)</f>
+        <f t="shared" si="0"/>
         <v>6791</v>
       </c>
       <c r="G10">
@@ -714,7 +725,7 @@
         <v>137700</v>
       </c>
       <c r="F11">
-        <f>F10+(E11-E10)*(G10/100)</f>
+        <f t="shared" si="0"/>
         <v>10011</v>
       </c>
       <c r="G11">
@@ -744,7 +755,7 @@
         <v>188700</v>
       </c>
       <c r="F12">
-        <f>F11+(E12-E11)*(G11/100)</f>
+        <f t="shared" si="0"/>
         <v>15621</v>
       </c>
       <c r="G12">
@@ -774,7 +785,7 @@
         <v>254900</v>
       </c>
       <c r="F13">
-        <f>F12+(E13-E12)*(G12/100)</f>
+        <f t="shared" si="0"/>
         <v>23565</v>
       </c>
       <c r="G13">
@@ -893,7 +904,7 @@
         <v>36700</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17:F25" si="0">F16+(E17-E16)*(G16/100)</f>
+        <f t="shared" ref="F17:F25" si="1">F16+(E17-E16)*(G16/100)</f>
         <v>729</v>
       </c>
       <c r="G17">
@@ -923,7 +934,7 @@
         <v>47400</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1264</v>
       </c>
       <c r="G18">
@@ -953,7 +964,7 @@
         <v>61300</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2098</v>
       </c>
       <c r="G19">
@@ -983,7 +994,7 @@
         <v>92100</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4254</v>
       </c>
       <c r="G20">
@@ -1013,7 +1024,7 @@
         <v>122900</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6718</v>
       </c>
       <c r="G21">
@@ -1043,7 +1054,7 @@
         <v>169300</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10894</v>
       </c>
       <c r="G22">
@@ -1073,7 +1084,7 @@
         <v>224700</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16434</v>
       </c>
       <c r="G23">
@@ -1103,7 +1114,7 @@
         <v>284800</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23045</v>
       </c>
       <c r="G24">
@@ -1133,7 +1144,7 @@
         <v>354100</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31361</v>
       </c>
       <c r="G25">
@@ -2896,7 +2907,844 @@
         <v>115</v>
       </c>
     </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A86">
+        <v>2019</v>
+      </c>
+      <c r="B86" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>10000</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>5</v>
+      </c>
+      <c r="H86">
+        <v>100</v>
+      </c>
+      <c r="I86">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A87">
+        <v>2019</v>
+      </c>
+      <c r="B87" t="s">
+        <v>11</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>13000</v>
+      </c>
+      <c r="F87">
+        <f>F86+(E87-E86)*(G86/100)</f>
+        <v>150</v>
+      </c>
+      <c r="G87">
+        <v>6</v>
+      </c>
+      <c r="H87">
+        <v>100</v>
+      </c>
+      <c r="I87">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A88">
+        <v>2019</v>
+      </c>
+      <c r="B88" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>17000</v>
+      </c>
+      <c r="F88">
+        <f>F87+(E88-E87)*(G87/100)</f>
+        <v>390</v>
+      </c>
+      <c r="G88">
+        <v>7</v>
+      </c>
+      <c r="H88">
+        <v>100</v>
+      </c>
+      <c r="I88">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A89">
+        <v>2019</v>
+      </c>
+      <c r="B89" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>24000</v>
+      </c>
+      <c r="F89">
+        <f>F88+(E89-E88)*(G88/100)</f>
+        <v>880</v>
+      </c>
+      <c r="G89">
+        <v>8</v>
+      </c>
+      <c r="H89">
+        <v>100</v>
+      </c>
+      <c r="I89">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A90">
+        <v>2019</v>
+      </c>
+      <c r="B90" t="s">
+        <v>11</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>30000</v>
+      </c>
+      <c r="F90">
+        <f>F89+(E90-E89)*(G89/100)</f>
+        <v>1360</v>
+      </c>
+      <c r="G90">
+        <v>9</v>
+      </c>
+      <c r="H90">
+        <v>100</v>
+      </c>
+      <c r="I90">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A91">
+        <v>2019</v>
+      </c>
+      <c r="B91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>36000</v>
+      </c>
+      <c r="F91">
+        <f>F90+(E91-E90)*(G90/100)</f>
+        <v>1900</v>
+      </c>
+      <c r="G91">
+        <v>9.5</v>
+      </c>
+      <c r="H91">
+        <v>100</v>
+      </c>
+      <c r="I91">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A92">
+        <v>2019</v>
+      </c>
+      <c r="B92" t="s">
+        <v>11</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>50000</v>
+      </c>
+      <c r="F92">
+        <f t="shared" ref="F92:F93" si="2">F91+(E92-E91)*(G91/100)</f>
+        <v>3230</v>
+      </c>
+      <c r="G92">
+        <v>10</v>
+      </c>
+      <c r="H92">
+        <v>100</v>
+      </c>
+      <c r="I92">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A93">
+        <v>2019</v>
+      </c>
+      <c r="B93" t="s">
+        <v>11</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>70000</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="2"/>
+        <v>5230</v>
+      </c>
+      <c r="G93">
+        <v>10.5</v>
+      </c>
+      <c r="H93">
+        <v>100</v>
+      </c>
+      <c r="I93">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A94">
+        <v>2019</v>
+      </c>
+      <c r="B94" t="s">
+        <v>11</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <v>98000</v>
+      </c>
+      <c r="F94">
+        <f t="shared" ref="F94:F95" si="3">F93+(E94-E93)*(G93/100)</f>
+        <v>8170</v>
+      </c>
+      <c r="G94">
+        <v>11.5</v>
+      </c>
+      <c r="H94">
+        <v>100</v>
+      </c>
+      <c r="I94">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A95">
+        <v>2019</v>
+      </c>
+      <c r="B95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95">
+        <v>310000</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="3"/>
+        <v>32550</v>
+      </c>
+      <c r="G95">
+        <v>10.5</v>
+      </c>
+      <c r="H95">
+        <v>100</v>
+      </c>
+      <c r="I95">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A96">
+        <v>2018</v>
+      </c>
+      <c r="B96" t="s">
+        <v>11</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>10000</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>5</v>
+      </c>
+      <c r="H96">
+        <v>100</v>
+      </c>
+      <c r="I96">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A97">
+        <v>2018</v>
+      </c>
+      <c r="B97" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>13000</v>
+      </c>
+      <c r="F97">
+        <f>F96+(E97-E96)*(G96/100)</f>
+        <v>150</v>
+      </c>
+      <c r="G97">
+        <v>6</v>
+      </c>
+      <c r="H97">
+        <v>100</v>
+      </c>
+      <c r="I97">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A98">
+        <v>2018</v>
+      </c>
+      <c r="B98" t="s">
+        <v>11</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>17000</v>
+      </c>
+      <c r="F98">
+        <f>F97+(E98-E97)*(G97/100)</f>
+        <v>390</v>
+      </c>
+      <c r="G98">
+        <v>7</v>
+      </c>
+      <c r="H98">
+        <v>100</v>
+      </c>
+      <c r="I98">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A99">
+        <v>2018</v>
+      </c>
+      <c r="B99" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>24000</v>
+      </c>
+      <c r="F99">
+        <f>F98+(E99-E98)*(G98/100)</f>
+        <v>880</v>
+      </c>
+      <c r="G99">
+        <v>8</v>
+      </c>
+      <c r="H99">
+        <v>100</v>
+      </c>
+      <c r="I99">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A100">
+        <v>2018</v>
+      </c>
+      <c r="B100" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100">
+        <v>30000</v>
+      </c>
+      <c r="F100">
+        <f>F99+(E100-E99)*(G99/100)</f>
+        <v>1360</v>
+      </c>
+      <c r="G100">
+        <v>9</v>
+      </c>
+      <c r="H100">
+        <v>100</v>
+      </c>
+      <c r="I100">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A101">
+        <v>2018</v>
+      </c>
+      <c r="B101" t="s">
+        <v>11</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>36000</v>
+      </c>
+      <c r="F101">
+        <f>F100+(E101-E100)*(G100/100)</f>
+        <v>1900</v>
+      </c>
+      <c r="G101">
+        <v>9.5</v>
+      </c>
+      <c r="H101">
+        <v>100</v>
+      </c>
+      <c r="I101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A102">
+        <v>2018</v>
+      </c>
+      <c r="B102" t="s">
+        <v>11</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>50000</v>
+      </c>
+      <c r="F102">
+        <f t="shared" ref="F102:F105" si="4">F101+(E102-E101)*(G101/100)</f>
+        <v>3230</v>
+      </c>
+      <c r="G102">
+        <v>10</v>
+      </c>
+      <c r="H102">
+        <v>100</v>
+      </c>
+      <c r="I102">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A103">
+        <v>2018</v>
+      </c>
+      <c r="B103" t="s">
+        <v>11</v>
+      </c>
+      <c r="C103">
+        <v>1</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <v>70000</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="4"/>
+        <v>5230</v>
+      </c>
+      <c r="G103">
+        <v>10.5</v>
+      </c>
+      <c r="H103">
+        <v>100</v>
+      </c>
+      <c r="I103">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A104">
+        <v>2018</v>
+      </c>
+      <c r="B104" t="s">
+        <v>11</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <v>98000</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="4"/>
+        <v>8170</v>
+      </c>
+      <c r="G104">
+        <v>11.5</v>
+      </c>
+      <c r="H104">
+        <v>100</v>
+      </c>
+      <c r="I104">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A105">
+        <v>2018</v>
+      </c>
+      <c r="B105" t="s">
+        <v>11</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+      <c r="E105">
+        <v>310000</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="4"/>
+        <v>32550</v>
+      </c>
+      <c r="G105">
+        <v>10.5</v>
+      </c>
+      <c r="H105">
+        <v>100</v>
+      </c>
+      <c r="I105">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A106">
+        <v>2019</v>
+      </c>
+      <c r="B106" t="s">
+        <v>11</v>
+      </c>
+      <c r="C106">
+        <v>4</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="G106">
+        <v>0.75</v>
+      </c>
+      <c r="H106">
+        <v>100</v>
+      </c>
+      <c r="I106">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A107">
+        <v>2019</v>
+      </c>
+      <c r="B107" t="s">
+        <v>11</v>
+      </c>
+      <c r="C107">
+        <v>4</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <v>50000</v>
+      </c>
+      <c r="F107">
+        <f>F106+(E107-E106)*(G106/1000)</f>
+        <v>37.5</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
+      </c>
+      <c r="H107">
+        <v>100</v>
+      </c>
+      <c r="I107">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A108">
+        <v>2019</v>
+      </c>
+      <c r="B108" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108">
+        <v>4</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <v>100000</v>
+      </c>
+      <c r="F108">
+        <f>F107+(E108-E107)*(G107/1000)</f>
+        <v>87.5</v>
+      </c>
+      <c r="G108">
+        <v>1.25</v>
+      </c>
+      <c r="H108">
+        <v>100</v>
+      </c>
+      <c r="I108">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A109">
+        <v>2019</v>
+      </c>
+      <c r="B109" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109">
+        <v>4</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109">
+        <v>150000</v>
+      </c>
+      <c r="F109">
+        <f>F108+(E109-E108)*(G108/1000)</f>
+        <v>150</v>
+      </c>
+      <c r="G109">
+        <v>1</v>
+      </c>
+      <c r="H109">
+        <v>100</v>
+      </c>
+      <c r="I109">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A110">
+        <v>2018</v>
+      </c>
+      <c r="B110" t="s">
+        <v>11</v>
+      </c>
+      <c r="C110">
+        <v>4</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+      <c r="G110">
+        <v>0.75</v>
+      </c>
+      <c r="H110">
+        <v>100</v>
+      </c>
+      <c r="I110">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A111">
+        <v>2018</v>
+      </c>
+      <c r="B111" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111">
+        <v>4</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111">
+        <v>50000</v>
+      </c>
+      <c r="F111">
+        <f>F110+(E111-E110)*(G110/1000)</f>
+        <v>37.5</v>
+      </c>
+      <c r="G111">
+        <v>1</v>
+      </c>
+      <c r="H111">
+        <v>100</v>
+      </c>
+      <c r="I111">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A112">
+        <v>2018</v>
+      </c>
+      <c r="B112" t="s">
+        <v>11</v>
+      </c>
+      <c r="C112">
+        <v>4</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112">
+        <v>100000</v>
+      </c>
+      <c r="F112">
+        <f>F111+(E112-E111)*(G111/1000)</f>
+        <v>87.5</v>
+      </c>
+      <c r="G112">
+        <v>1.25</v>
+      </c>
+      <c r="H112">
+        <v>100</v>
+      </c>
+      <c r="I112">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A113">
+        <v>2018</v>
+      </c>
+      <c r="B113" t="s">
+        <v>11</v>
+      </c>
+      <c r="C113">
+        <v>4</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113">
+        <v>150000</v>
+      </c>
+      <c r="F113">
+        <f>F112+(E113-E112)*(G112/1000)</f>
+        <v>150</v>
+      </c>
+      <c r="G113">
+        <v>1</v>
+      </c>
+      <c r="H113">
+        <v>100</v>
+      </c>
+      <c r="I113">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add canton tax rate for SO
</commit_message>
<xml_diff>
--- a/data/Steuertarife.xlsx
+++ b/data/Steuertarife.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\PensionTools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC7CDEA-ED05-409F-A561-016A74DC58D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2403A7B-69A0-418D-AA31-424F1AAB28B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="K106" sqref="K106"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="I105" sqref="I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2933,7 +2933,7 @@
         <v>100</v>
       </c>
       <c r="I86">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.75">
@@ -2963,7 +2963,7 @@
         <v>100</v>
       </c>
       <c r="I87">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.75">
@@ -2993,7 +2993,7 @@
         <v>100</v>
       </c>
       <c r="I88">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.75">
@@ -3023,7 +3023,7 @@
         <v>100</v>
       </c>
       <c r="I89">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.75">
@@ -3053,7 +3053,7 @@
         <v>100</v>
       </c>
       <c r="I90">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.75">
@@ -3083,7 +3083,7 @@
         <v>100</v>
       </c>
       <c r="I91">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.75">
@@ -3113,7 +3113,7 @@
         <v>100</v>
       </c>
       <c r="I92">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.75">
@@ -3143,7 +3143,7 @@
         <v>100</v>
       </c>
       <c r="I93">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.75">
@@ -3173,7 +3173,7 @@
         <v>100</v>
       </c>
       <c r="I94">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.75">
@@ -3203,7 +3203,7 @@
         <v>100</v>
       </c>
       <c r="I95">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.75">
@@ -3232,7 +3232,7 @@
         <v>100</v>
       </c>
       <c r="I96">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.75">
@@ -3262,7 +3262,7 @@
         <v>100</v>
       </c>
       <c r="I97">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.75">
@@ -3292,7 +3292,7 @@
         <v>100</v>
       </c>
       <c r="I98">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.75">
@@ -3322,7 +3322,7 @@
         <v>100</v>
       </c>
       <c r="I99">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.75">
@@ -3352,7 +3352,7 @@
         <v>100</v>
       </c>
       <c r="I100">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.75">
@@ -3382,7 +3382,7 @@
         <v>100</v>
       </c>
       <c r="I101">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.75">
@@ -3412,7 +3412,7 @@
         <v>100</v>
       </c>
       <c r="I102">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.75">
@@ -3442,7 +3442,7 @@
         <v>100</v>
       </c>
       <c r="I103">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.75">
@@ -3472,7 +3472,7 @@
         <v>100</v>
       </c>
       <c r="I104">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.75">
@@ -3502,7 +3502,7 @@
         <v>100</v>
       </c>
       <c r="I105">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
add income tax calculator
</commit_message>
<xml_diff>
--- a/data/Steuertarife.xlsx
+++ b/data/Steuertarife.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\PensionTools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2403A7B-69A0-418D-AA31-424F1AAB28B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF12E44-CD00-4E24-BA08-A0561804285E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="I105" sqref="I105"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="N90" sqref="N90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2930,7 +2930,7 @@
         <v>5</v>
       </c>
       <c r="H86">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I86">
         <v>104</v>
@@ -2960,7 +2960,7 @@
         <v>6</v>
       </c>
       <c r="H87">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I87">
         <v>104</v>
@@ -2990,7 +2990,7 @@
         <v>7</v>
       </c>
       <c r="H88">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I88">
         <v>104</v>
@@ -3020,7 +3020,7 @@
         <v>8</v>
       </c>
       <c r="H89">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I89">
         <v>104</v>
@@ -3050,7 +3050,7 @@
         <v>9</v>
       </c>
       <c r="H90">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I90">
         <v>104</v>
@@ -3080,7 +3080,7 @@
         <v>9.5</v>
       </c>
       <c r="H91">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I91">
         <v>104</v>
@@ -3110,7 +3110,7 @@
         <v>10</v>
       </c>
       <c r="H92">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I92">
         <v>104</v>
@@ -3140,7 +3140,7 @@
         <v>10.5</v>
       </c>
       <c r="H93">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I93">
         <v>104</v>
@@ -3170,7 +3170,7 @@
         <v>11.5</v>
       </c>
       <c r="H94">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I94">
         <v>104</v>
@@ -3200,7 +3200,7 @@
         <v>10.5</v>
       </c>
       <c r="H95">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I95">
         <v>104</v>
@@ -3229,7 +3229,7 @@
         <v>5</v>
       </c>
       <c r="H96">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I96">
         <v>104</v>
@@ -3259,7 +3259,7 @@
         <v>6</v>
       </c>
       <c r="H97">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I97">
         <v>104</v>
@@ -3289,7 +3289,7 @@
         <v>7</v>
       </c>
       <c r="H98">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I98">
         <v>104</v>
@@ -3319,7 +3319,7 @@
         <v>8</v>
       </c>
       <c r="H99">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I99">
         <v>104</v>
@@ -3349,7 +3349,7 @@
         <v>9</v>
       </c>
       <c r="H100">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I100">
         <v>104</v>
@@ -3379,7 +3379,7 @@
         <v>9.5</v>
       </c>
       <c r="H101">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I101">
         <v>104</v>
@@ -3409,7 +3409,7 @@
         <v>10</v>
       </c>
       <c r="H102">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I102">
         <v>104</v>
@@ -3439,7 +3439,7 @@
         <v>10.5</v>
       </c>
       <c r="H103">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I103">
         <v>104</v>
@@ -3469,7 +3469,7 @@
         <v>11.5</v>
       </c>
       <c r="H104">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I104">
         <v>104</v>
@@ -3499,7 +3499,7 @@
         <v>10.5</v>
       </c>
       <c r="H105">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I105">
         <v>104</v>
@@ -3528,7 +3528,7 @@
         <v>0.75</v>
       </c>
       <c r="H106">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I106">
         <v>100</v>
@@ -3558,7 +3558,7 @@
         <v>1</v>
       </c>
       <c r="H107">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I107">
         <v>100</v>
@@ -3588,7 +3588,7 @@
         <v>1.25</v>
       </c>
       <c r="H108">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I108">
         <v>100</v>
@@ -3618,7 +3618,7 @@
         <v>1</v>
       </c>
       <c r="H109">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I109">
         <v>100</v>
@@ -3647,7 +3647,7 @@
         <v>0.75</v>
       </c>
       <c r="H110">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I110">
         <v>100</v>
@@ -3677,7 +3677,7 @@
         <v>1</v>
       </c>
       <c r="H111">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I111">
         <v>100</v>
@@ -3707,7 +3707,7 @@
         <v>1.25</v>
       </c>
       <c r="H112">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I112">
         <v>100</v>
@@ -3737,7 +3737,7 @@
         <v>1</v>
       </c>
       <c r="H113">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I113">
         <v>100</v>

</xml_diff>